<commit_message>
Added 29 COVID-19 diagnostic kits made in China
Added 29 COVID-19 diagnostic kits made in China

Yujia Tian and Oliver He
</commit_message>
<xml_diff>
--- a/src/ontology/Ontorat input/China diagnosis kits EUA/China_diagnosis_kits_in_English.xlsx
+++ b/src/ontology/Ontorat input/China diagnosis kits EUA/China_diagnosis_kits_in_English.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yongqunh\GitHub\cido\src\ontology\Ontorat input\China diagnosis kits EUA\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42A065ED-E6E7-4DE5-B7E4-65EDE6F3C255}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="218">
   <si>
     <t>Product name</t>
   </si>
@@ -260,9 +269,6 @@
     <t>Store below -18°C away from light, valid for 6 months.</t>
   </si>
   <si>
-    <t>SARS-CoV-2 detection using quantum dot fluorescence immunochromatography combined with isothermal amplification and CRISPR/Cas13a.</t>
-  </si>
-  <si>
     <t>Hangzhou Zhongce Biotechnology Co., Ltd.</t>
   </si>
   <si>
@@ -449,9 +455,6 @@
     <t>Store at 2~30°C in a dry place away from light and heat. The validity period of the kit is tentatively set for 6 months.</t>
   </si>
   <si>
-    <t xml:space="preserve">SARS-CoV-2 Nucleic Acid Detection Kit RNA  (RNA isothermal amplification-gold probe chromatography) </t>
-  </si>
-  <si>
     <t>Wuhan Zhongzhi Biotechnologies INC.</t>
   </si>
   <si>
@@ -470,9 +473,6 @@
     <t>Box A is stored at -40℃～-15℃, and box B is stored at 2～30℃. The validity period of the kit is 9 months.</t>
   </si>
   <si>
-    <t xml:space="preserve"> SARS-CoV-2 Nucleic Acid Detection Kit RNA (combined probe-anchored polymerization sequencing method)</t>
-  </si>
-  <si>
     <t>NO.20203400059</t>
   </si>
   <si>
@@ -591,64 +591,157 @@
   </si>
   <si>
     <t>Store below -15°C away from light, valid for 11 months.</t>
+  </si>
+  <si>
+    <t>中山大学达安基因股份有限公司</t>
+  </si>
+  <si>
+    <t>浙江东方基因生物制品股份有限公司</t>
+  </si>
+  <si>
+    <t>上海复星长征医学科学有限公司</t>
+  </si>
+  <si>
+    <t>武汉中帜生物科技股份有限公司</t>
+  </si>
+  <si>
+    <t>北京金豪制药股份有限公司</t>
+  </si>
+  <si>
+    <t>上海伯杰医疗科技有限公司</t>
+  </si>
+  <si>
+    <t>江苏硕世生物科技股份有限公司</t>
+  </si>
+  <si>
+    <t>迈克生物股份有限公司</t>
+  </si>
+  <si>
+    <t>上海捷诺生物科技有限公司</t>
+  </si>
+  <si>
+    <t>上海之江生物科技股份有限公司</t>
+  </si>
+  <si>
+    <t>华大生物科技（武汉）有限公司</t>
+  </si>
+  <si>
+    <t>杭州众测生物科技有限公司</t>
+  </si>
+  <si>
+    <t>卡尤迪生物科技宜兴有限公司</t>
+  </si>
+  <si>
+    <t>圣湘生物科技股份有限公司</t>
+  </si>
+  <si>
+    <t>北京卓诚惠生生物科技股份有限公司</t>
+  </si>
+  <si>
+    <t>北京纳捷诊断试剂有限公司</t>
+  </si>
+  <si>
+    <t>深圳联合医学科技有限公司</t>
+  </si>
+  <si>
+    <t>武汉明德生物科技股份有限公司</t>
+  </si>
+  <si>
+    <t>上海仁度生物科技股份有限公司</t>
+  </si>
+  <si>
+    <t>安邦（厦门）生物科技有限公司</t>
+  </si>
+  <si>
+    <t>成都博奥晶芯生物科技有限公司</t>
+  </si>
+  <si>
+    <t>杭州优思达生物技术有限公司</t>
+  </si>
+  <si>
+    <t>杭州迪安生物技术有限公司</t>
+  </si>
+  <si>
+    <t>重庆中元汇吉生物技术有限公司</t>
+  </si>
+  <si>
+    <t>潮州凯普生物化学有限公司</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2 Nucleic Acid Detection Kit (CRISPR immunochromatography)</t>
+  </si>
+  <si>
+    <t>SARS-CoV-2 Nucleic Acid Detection Kit RNA (combined probe-anchored polymerization sequencing method)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SARS-CoV-2 Nucleic Acid Detection Kit RNA (RNA isothermal amplification-gold probe chromatography) </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
+      <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -659,7 +752,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -669,81 +762,82 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" readingOrder="0" vertical="top"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -933,1178 +1027,1272 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:M61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="20.88"/>
-    <col customWidth="1" min="2" max="2" width="19.13"/>
-    <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="4" width="14.88"/>
-    <col customWidth="1" min="6" max="6" width="47.75"/>
-    <col customWidth="1" min="7" max="7" width="40.5"/>
-    <col customWidth="1" min="8" max="8" width="36.63"/>
-    <col customWidth="1" min="9" max="9" width="15.0"/>
-    <col customWidth="1" min="10" max="10" width="27.5"/>
+    <col min="1" max="1" width="94.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" customWidth="1"/>
+    <col min="7" max="7" width="47.7109375" customWidth="1"/>
+    <col min="8" max="8" width="40.42578125" customWidth="1"/>
+    <col min="9" max="9" width="36.5703125" customWidth="1"/>
+    <col min="10" max="10" width="15" customWidth="1"/>
+    <col min="11" max="11" width="27.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5"/>
-    </row>
-    <row r="2">
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="9">
-        <v>44095.0</v>
-      </c>
       <c r="E2" s="9">
-        <v>44459.0</v>
-      </c>
-      <c r="F2" s="10" t="s">
+        <v>44095</v>
+      </c>
+      <c r="F2" s="9">
+        <v>44459</v>
+      </c>
+      <c r="G2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="L2" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="9">
-        <v>44249.0</v>
-      </c>
-      <c r="E3" s="12">
-        <v>46074.0</v>
-      </c>
-      <c r="F3" s="13" t="s">
+      <c r="E3" s="9">
+        <v>44249</v>
+      </c>
+      <c r="F3" s="12">
+        <v>46074</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="11" t="s">
+      <c r="H3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="I3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="11" t="s">
+      <c r="K3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="L3" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" t="s">
+        <v>192</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="9">
-        <v>44217.0</v>
-      </c>
-      <c r="E4" s="12">
-        <v>46042.0</v>
-      </c>
-      <c r="F4" s="13" t="s">
+      <c r="E4" s="9">
+        <v>44217</v>
+      </c>
+      <c r="F4" s="12">
+        <v>46042</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="G4" s="6" t="s">
+      <c r="H4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="I4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="K4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="L4" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
         <v>31</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="9">
-        <v>44234.0</v>
-      </c>
-      <c r="E5" s="12">
-        <v>46059.0</v>
-      </c>
-      <c r="F5" s="13" t="s">
+      <c r="E5" s="9">
+        <v>44234</v>
+      </c>
+      <c r="F5" s="12">
+        <v>46059</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="K5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6">
+      <c r="L5" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="9">
-        <v>43924.0</v>
-      </c>
-      <c r="E6" s="12">
-        <v>46092.0</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="9">
+        <v>43924</v>
+      </c>
+      <c r="F6" s="12">
+        <v>46092</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="H6" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="I6" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="J6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J6" s="11" t="s">
+      <c r="K6" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="K6" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7">
+      <c r="L6" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" t="s">
+        <v>195</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="9">
-        <v>44207.0</v>
-      </c>
-      <c r="E7" s="12">
-        <v>46032.0</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="9">
+        <v>44207</v>
+      </c>
+      <c r="F7" s="12">
+        <v>46032</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="H7" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="J7" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="11" t="s">
+      <c r="K7" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8">
+      <c r="L7" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" t="s">
+        <v>196</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="9">
-        <v>44155.0</v>
-      </c>
-      <c r="E8" s="12">
-        <v>45980.0</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="9">
+        <v>44155</v>
+      </c>
+      <c r="F8" s="12">
+        <v>45980</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="H8" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="K8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9">
+      <c r="L8" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" t="s">
+        <v>197</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="9">
-        <v>44237.0</v>
-      </c>
-      <c r="E9" s="12">
-        <v>46062.0</v>
-      </c>
-      <c r="F9" s="13" t="s">
+      <c r="E9" s="9">
+        <v>44237</v>
+      </c>
+      <c r="F9" s="12">
+        <v>46062</v>
+      </c>
+      <c r="G9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="H9" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="J9" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="K9" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="K9" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10">
+      <c r="L9" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" t="s">
+        <v>198</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="D10" s="9">
-        <v>44155.0</v>
-      </c>
-      <c r="E10" s="12">
-        <v>45980.0</v>
-      </c>
-      <c r="F10" s="13" t="s">
+      <c r="E10" s="9">
+        <v>44155</v>
+      </c>
+      <c r="F10" s="12">
+        <v>45980</v>
+      </c>
+      <c r="G10" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="J10" s="8" t="s">
+      <c r="K10" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="K10" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="L10" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" t="s">
+        <v>199</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="9">
-        <v>44204.0</v>
-      </c>
-      <c r="E11" s="12">
-        <v>46029.0</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="E11" s="9">
+        <v>44204</v>
+      </c>
+      <c r="F11" s="12">
+        <v>46029</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="11" t="s">
+      <c r="H11" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="I11" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="I11" s="13" t="s">
+      <c r="J11" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="K11" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12">
+      <c r="L11" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" t="s">
+        <v>200</v>
+      </c>
+      <c r="D12" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="9">
-        <v>44201.0</v>
-      </c>
-      <c r="E12" s="12">
-        <v>46026.0</v>
-      </c>
-      <c r="F12" s="13" t="s">
+      <c r="E12" s="9">
+        <v>44201</v>
+      </c>
+      <c r="F12" s="12">
+        <v>46026</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="G12" s="11" t="s">
+      <c r="H12" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="I12" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="K12" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="K12" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="6" t="s">
+      <c r="L12" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="11" t="s">
+        <v>215</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D13" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="E13" s="9">
+        <v>44165</v>
+      </c>
+      <c r="F13" s="9">
+        <v>44529</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="D13" s="9">
-        <v>44165.0</v>
-      </c>
-      <c r="E13" s="9">
-        <v>44529.0</v>
-      </c>
-      <c r="F13" s="10" t="s">
+      <c r="H13" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="G13" s="11" t="s">
+      <c r="I13" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="J13" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="I13" s="16" t="s">
+      <c r="K13" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="J13" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="K13" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14">
+      <c r="L13" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" t="s">
+        <v>202</v>
+      </c>
+      <c r="D14" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="E14" s="9">
+        <v>44025</v>
+      </c>
+      <c r="F14" s="9">
+        <v>44389</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="D14" s="9">
-        <v>44025.0</v>
-      </c>
-      <c r="E14" s="9">
-        <v>44389.0</v>
-      </c>
-      <c r="F14" s="13" t="s">
+      <c r="H14" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="G14" s="11" t="s">
+      <c r="I14" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="K14" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="J14" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="K14" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15">
+      <c r="L14" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="C15" t="s">
+        <v>203</v>
+      </c>
+      <c r="D15" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="E15" s="9">
+        <v>44223</v>
+      </c>
+      <c r="F15" s="12">
+        <v>46048</v>
+      </c>
+      <c r="G15" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="9">
-        <v>44223.0</v>
-      </c>
-      <c r="E15" s="12">
-        <v>46048.0</v>
-      </c>
-      <c r="F15" s="13" t="s">
+      <c r="H15" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="G15" s="11" t="s">
+      <c r="I15" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="H15" s="11" t="s">
+      <c r="J15" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="K15" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="J15" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="K15" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16">
+      <c r="L15" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" t="s">
+        <v>190</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="9">
+        <v>44217</v>
+      </c>
+      <c r="F16" s="12">
+        <v>46042</v>
+      </c>
+      <c r="G16" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="9">
-        <v>44217.0</v>
-      </c>
-      <c r="E16" s="12">
-        <v>46042.0</v>
-      </c>
-      <c r="F16" s="13" t="s">
+      <c r="H16" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="I16" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="K16" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="J16" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="K16" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17">
+      <c r="L16" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C17" t="s">
+        <v>204</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="E17" s="17">
+        <v>44251</v>
+      </c>
+      <c r="F17" s="12">
+        <v>46076</v>
+      </c>
+      <c r="G17" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="D17" s="17">
-        <v>44251.0</v>
-      </c>
-      <c r="E17" s="12">
-        <v>46076.0</v>
-      </c>
-      <c r="F17" s="13" t="s">
+      <c r="H17" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="G17" s="11" t="s">
+      <c r="I17" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="H17" s="11" t="s">
+      <c r="K17" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="J17" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="K17" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18">
+      <c r="L17" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C18" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="E18" s="9">
+        <v>43991</v>
+      </c>
+      <c r="F18" s="9">
+        <v>44355</v>
+      </c>
+      <c r="G18" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="D18" s="9">
-        <v>43991.0</v>
-      </c>
-      <c r="E18" s="9">
-        <v>44355.0</v>
-      </c>
-      <c r="F18" s="13" t="s">
+      <c r="H18" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="G18" s="11" t="s">
+      <c r="I18" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="H18" s="11" t="s">
+      <c r="K18" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="J18" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="K18" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19">
+      <c r="L18" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C19" t="s">
+        <v>206</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="E19" s="9">
+        <v>43987</v>
+      </c>
+      <c r="F19" s="9">
+        <v>44351</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="D19" s="9">
-        <v>43987.0</v>
-      </c>
-      <c r="E19" s="9">
-        <v>44351.0</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="H19" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="G19" s="11" t="s">
+      <c r="I19" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="H19" s="11" t="s">
+      <c r="K19" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="J19" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="K19" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20">
+      <c r="L19" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="C20" t="s">
+        <v>207</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="E20" s="17">
+        <v>44237</v>
+      </c>
+      <c r="F20" s="12">
+        <v>46062</v>
+      </c>
+      <c r="G20" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="D20" s="17">
-        <v>44237.0</v>
-      </c>
-      <c r="E20" s="12">
-        <v>46062.0</v>
-      </c>
-      <c r="F20" s="13" t="s">
+      <c r="H20" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="G20" s="11" t="s">
+      <c r="I20" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="H20" s="11" t="s">
+      <c r="K20" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="J20" s="11" t="s">
+      <c r="L20" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A21" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="K20" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="11" t="s">
+      <c r="B21" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="C21" t="s">
+        <v>208</v>
+      </c>
+      <c r="D21" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="E21" s="17">
+        <v>44236</v>
+      </c>
+      <c r="F21" s="12">
+        <v>46061</v>
+      </c>
+      <c r="G21" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="17">
-        <v>44236.0</v>
-      </c>
-      <c r="E21" s="12">
-        <v>46061.0</v>
-      </c>
-      <c r="F21" s="13" t="s">
+      <c r="H21" s="11" t="s">
         <v>135</v>
       </c>
-      <c r="G21" s="11" t="s">
+      <c r="I21" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="11" t="s">
+      <c r="K21" s="11" t="s">
         <v>137</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="L21" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A22" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="K21" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="11" t="s">
+      <c r="B22" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" t="s">
+        <v>209</v>
+      </c>
+      <c r="D22" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="E22" s="9">
+        <v>43914</v>
+      </c>
+      <c r="F22" s="9">
+        <v>44278</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="D22" s="9">
-        <v>43914.0</v>
-      </c>
-      <c r="E22" s="9">
-        <v>44278.0</v>
-      </c>
-      <c r="F22" s="13" t="s">
+      <c r="H22" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="I22" s="11" t="s">
         <v>142</v>
       </c>
-      <c r="G22" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="H22" s="11" t="s">
+      <c r="K22" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="L22" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A23" s="11" t="s">
+        <v>217</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="K22" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="11" t="s">
+      <c r="C23" t="s">
+        <v>193</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="E23" s="9">
+        <v>44234</v>
+      </c>
+      <c r="F23" s="12">
+        <v>46059</v>
+      </c>
+      <c r="G23" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="H23" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="9">
-        <v>44234.0</v>
-      </c>
-      <c r="E23" s="12">
-        <v>46059.0</v>
-      </c>
-      <c r="F23" s="13" t="s">
+      <c r="I23" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="K23" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="H23" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="J23" s="11" t="s">
-        <v>151</v>
-      </c>
-      <c r="K23" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24">
+      <c r="L23" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
-        <v>152</v>
+        <v>216</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" t="s">
+        <v>200</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="9">
+        <v>44201</v>
+      </c>
+      <c r="F24" s="12">
+        <v>46026</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="H24" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="I24" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="D24" s="9">
-        <v>44201.0</v>
-      </c>
-      <c r="E24" s="12">
-        <v>46026.0</v>
-      </c>
-      <c r="F24" s="10" t="s">
+      <c r="K24" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="L24" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A25" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="H24" s="8" t="s">
+      <c r="B25" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="J24" s="11" t="s">
+      <c r="C25" t="s">
+        <v>210</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="K24" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="11" t="s">
+      <c r="E25" s="9">
+        <v>44236</v>
+      </c>
+      <c r="F25" s="9">
+        <v>44600</v>
+      </c>
+      <c r="G25" s="13" t="s">
         <v>158</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="H25" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="I25" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="D25" s="9">
-        <v>44236.0</v>
-      </c>
-      <c r="E25" s="9">
-        <v>44600.0</v>
-      </c>
-      <c r="F25" s="13" t="s">
+      <c r="K25" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="L25" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="H25" s="11" t="s">
+      <c r="B26" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="J25" s="11" t="s">
+      <c r="C26" t="s">
+        <v>211</v>
+      </c>
+      <c r="D26" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="K25" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="11" t="s">
+      <c r="E26" s="9">
+        <v>44201</v>
+      </c>
+      <c r="F26" s="12">
+        <v>46026</v>
+      </c>
+      <c r="G26" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="H26" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="K26" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="D26" s="9">
-        <v>44201.0</v>
-      </c>
-      <c r="E26" s="12">
-        <v>46026.0</v>
-      </c>
-      <c r="F26" s="13" t="s">
+      <c r="L26" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="G26" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H26" s="11" t="s">
+      <c r="B27" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="C27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="E27" s="9">
+        <v>43883</v>
+      </c>
+      <c r="F27" s="9">
+        <v>44248</v>
+      </c>
+      <c r="G27" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="K26" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="11" t="s">
+      <c r="H27" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="B27" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="C27" s="8" t="s">
+      <c r="I27" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="D27" s="9">
-        <v>43883.0</v>
-      </c>
-      <c r="E27" s="9">
-        <v>44248.0</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>173</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>174</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>175</v>
-      </c>
-      <c r="J27" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28">
+      <c r="K27" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="L27" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B28" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="C28" t="s">
+        <v>212</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E28" s="9">
+        <v>44273</v>
+      </c>
+      <c r="F28" s="12">
+        <v>46098</v>
+      </c>
+      <c r="G28" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="H28" s="11" t="s">
         <v>176</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="I28" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D28" s="9">
-        <v>44273.0</v>
-      </c>
-      <c r="E28" s="12">
-        <v>46098.0</v>
-      </c>
-      <c r="F28" s="13" t="s">
+      <c r="K28" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="G28" s="11" t="s">
-        <v>179</v>
-      </c>
-      <c r="H28" s="11" t="s">
-        <v>180</v>
-      </c>
-      <c r="J28" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29">
+      <c r="L28" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="C29" t="s">
+        <v>213</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="E29" s="9">
+        <v>44287</v>
+      </c>
+      <c r="F29" s="12">
+        <v>46112</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="H29" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="I29" s="11" t="s">
         <v>183</v>
       </c>
-      <c r="D29" s="9">
-        <v>44287.0</v>
-      </c>
-      <c r="E29" s="12">
-        <v>46112.0</v>
-      </c>
-      <c r="F29" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>186</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30">
+      <c r="K29" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="L29" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B30" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="C30" t="s">
+        <v>214</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>185</v>
+      </c>
+      <c r="E30" s="9">
+        <v>44295</v>
+      </c>
+      <c r="F30" s="12">
+        <v>46120</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="H30" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="I30" s="11" t="s">
         <v>188</v>
       </c>
-      <c r="D30" s="9">
-        <v>44295.0</v>
-      </c>
-      <c r="E30" s="12">
-        <v>46120.0</v>
-      </c>
-      <c r="F30" s="13" t="s">
+      <c r="K30" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="G30" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="H30" s="11" t="s">
-        <v>191</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>192</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="D31" s="18"/>
+      <c r="L30" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E31" s="18"/>
-    </row>
-    <row r="32">
-      <c r="D32" s="18"/>
+      <c r="F31" s="18"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E32" s="18"/>
-    </row>
-    <row r="33">
-      <c r="D33" s="18"/>
+      <c r="F32" s="18"/>
+    </row>
+    <row r="33" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E33" s="18"/>
-    </row>
-    <row r="34">
-      <c r="D34" s="18"/>
+      <c r="F33" s="18"/>
+    </row>
+    <row r="34" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E34" s="18"/>
-    </row>
-    <row r="35">
-      <c r="D35" s="18"/>
+      <c r="F34" s="18"/>
+    </row>
+    <row r="35" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E35" s="18"/>
-    </row>
-    <row r="36">
-      <c r="D36" s="18"/>
+      <c r="F35" s="18"/>
+    </row>
+    <row r="36" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E36" s="18"/>
-    </row>
-    <row r="37">
-      <c r="D37" s="18"/>
+      <c r="F36" s="18"/>
+    </row>
+    <row r="37" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E37" s="18"/>
-    </row>
-    <row r="38">
-      <c r="D38" s="18"/>
+      <c r="F37" s="18"/>
+    </row>
+    <row r="38" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E38" s="18"/>
-    </row>
-    <row r="39">
-      <c r="D39" s="18"/>
+      <c r="F38" s="18"/>
+    </row>
+    <row r="39" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E39" s="18"/>
-    </row>
-    <row r="40">
-      <c r="D40" s="18"/>
+      <c r="F39" s="18"/>
+    </row>
+    <row r="40" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E40" s="18"/>
-    </row>
-    <row r="41">
-      <c r="D41" s="18"/>
+      <c r="F40" s="18"/>
+    </row>
+    <row r="41" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E41" s="18"/>
-    </row>
-    <row r="42">
-      <c r="D42" s="18"/>
+      <c r="F41" s="18"/>
+    </row>
+    <row r="42" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E42" s="18"/>
-    </row>
-    <row r="43">
-      <c r="D43" s="18"/>
+      <c r="F42" s="18"/>
+    </row>
+    <row r="43" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E43" s="18"/>
-    </row>
-    <row r="44">
-      <c r="D44" s="18"/>
+      <c r="F43" s="18"/>
+    </row>
+    <row r="44" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E44" s="18"/>
-    </row>
-    <row r="45">
-      <c r="D45" s="18"/>
+      <c r="F44" s="18"/>
+    </row>
+    <row r="45" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E45" s="18"/>
-    </row>
-    <row r="46">
-      <c r="D46" s="18"/>
+      <c r="F45" s="18"/>
+    </row>
+    <row r="46" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E46" s="18"/>
-    </row>
-    <row r="47">
-      <c r="D47" s="18"/>
+      <c r="F46" s="18"/>
+    </row>
+    <row r="47" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E47" s="18"/>
-    </row>
-    <row r="48">
-      <c r="D48" s="18"/>
+      <c r="F47" s="18"/>
+    </row>
+    <row r="48" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E48" s="18"/>
-    </row>
-    <row r="49">
-      <c r="D49" s="18"/>
+      <c r="F48" s="18"/>
+    </row>
+    <row r="49" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E49" s="18"/>
-    </row>
-    <row r="50">
-      <c r="D50" s="18"/>
+      <c r="F49" s="18"/>
+    </row>
+    <row r="50" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E50" s="18"/>
-    </row>
-    <row r="51">
-      <c r="D51" s="18"/>
+      <c r="F50" s="18"/>
+    </row>
+    <row r="51" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E51" s="18"/>
-    </row>
-    <row r="52">
-      <c r="D52" s="18"/>
+      <c r="F51" s="18"/>
+    </row>
+    <row r="52" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E52" s="18"/>
-    </row>
-    <row r="53">
-      <c r="D53" s="18"/>
+      <c r="F52" s="18"/>
+    </row>
+    <row r="53" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E53" s="18"/>
-    </row>
-    <row r="54">
-      <c r="D54" s="18"/>
+      <c r="F53" s="18"/>
+    </row>
+    <row r="54" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E54" s="18"/>
-    </row>
-    <row r="55">
-      <c r="D55" s="18"/>
+      <c r="F54" s="18"/>
+    </row>
+    <row r="55" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E55" s="18"/>
-    </row>
-    <row r="56">
-      <c r="D56" s="18"/>
+      <c r="F55" s="18"/>
+    </row>
+    <row r="56" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E56" s="18"/>
-    </row>
-    <row r="57">
-      <c r="D57" s="18"/>
+      <c r="F56" s="18"/>
+    </row>
+    <row r="57" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E57" s="18"/>
-    </row>
-    <row r="58">
-      <c r="D58" s="18"/>
+      <c r="F57" s="18"/>
+    </row>
+    <row r="58" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E58" s="18"/>
-    </row>
-    <row r="59">
-      <c r="D59" s="18"/>
+      <c r="F58" s="18"/>
+    </row>
+    <row r="59" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E59" s="18"/>
-    </row>
-    <row r="60">
-      <c r="D60" s="18"/>
+      <c r="F59" s="18"/>
+    </row>
+    <row r="60" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E60" s="18"/>
-    </row>
-    <row r="61">
-      <c r="D61" s="18"/>
+      <c r="F60" s="18"/>
+    </row>
+    <row r="61" spans="5:6" x14ac:dyDescent="0.2">
       <c r="E61" s="18"/>
+      <c r="F61" s="18"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="I2"/>
-    <hyperlink r:id="rId3" ref="F3"/>
-    <hyperlink r:id="rId4" ref="F4"/>
-    <hyperlink r:id="rId5" ref="F5"/>
-    <hyperlink r:id="rId6" ref="F6"/>
-    <hyperlink r:id="rId7" ref="I6"/>
-    <hyperlink r:id="rId8" ref="F7"/>
-    <hyperlink r:id="rId9" ref="I7"/>
-    <hyperlink r:id="rId10" ref="F8"/>
-    <hyperlink r:id="rId11" ref="F9"/>
-    <hyperlink r:id="rId12" ref="I9"/>
-    <hyperlink r:id="rId13" ref="F10"/>
-    <hyperlink r:id="rId14" ref="F11"/>
-    <hyperlink r:id="rId15" ref="I11"/>
-    <hyperlink r:id="rId16" ref="F12"/>
-    <hyperlink r:id="rId17" ref="F13"/>
-    <hyperlink r:id="rId18" ref="I13"/>
-    <hyperlink r:id="rId19" ref="F14"/>
-    <hyperlink r:id="rId20" ref="F15"/>
-    <hyperlink r:id="rId21" ref="I15"/>
-    <hyperlink r:id="rId22" ref="F16"/>
-    <hyperlink r:id="rId23" ref="F17"/>
-    <hyperlink r:id="rId24" ref="F18"/>
-    <hyperlink r:id="rId25" ref="F19"/>
-    <hyperlink r:id="rId26" ref="F20"/>
-    <hyperlink r:id="rId27" ref="F21"/>
-    <hyperlink r:id="rId28" ref="F22"/>
-    <hyperlink r:id="rId29" ref="F23"/>
-    <hyperlink r:id="rId30" ref="F24"/>
-    <hyperlink r:id="rId31" ref="F25"/>
-    <hyperlink r:id="rId32" ref="F26"/>
-    <hyperlink r:id="rId33" ref="F27"/>
-    <hyperlink r:id="rId34" ref="F28"/>
-    <hyperlink r:id="rId35" ref="F29"/>
-    <hyperlink r:id="rId36" ref="F30"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="J2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="G3" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="G4" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="G5" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="G6" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="J6" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="G7" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J7" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="G8" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="G9" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J9" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="G10" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="G11" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J11" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="G12" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="G13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J13" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="G14" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="G15" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="J15" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="G16" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="G17" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="G18" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="G19" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="G20" r:id="rId26" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="G21" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="G22" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="G23" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="G24" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="G25" r:id="rId31" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="G26" r:id="rId32" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="G27" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="G28" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="G29" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="G30" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
   </hyperlinks>
-  <drawing r:id="rId37"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>